<commit_message>
Changes in flowchart diagram
</commit_message>
<xml_diff>
--- a/Lab03/Docs/Lab03_WBT_TCs_Form.xlsx
+++ b/Lab03/Docs/Lab03_WBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="459" documentId="11_6DFBBE858289C8C7F32634D05F6B97BC65B49737" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10313389-3D61-44FF-A32F-9CA41385E639}"/>
+  <xr:revisionPtr revIDLastSave="554" documentId="11_6DFBBE858289C8C7F32634D05F6B97BC65B49737" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D177F855-427C-4630-8EE6-F559F7A9FCC9}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="169">
   <si>
     <t>Informaţiile vor fi preluate din fişiere text.</t>
   </si>
@@ -546,21 +546,12 @@
     <t>sb.append(time[k]);</t>
   </si>
   <si>
-    <t>sb.append(time[k] &gt; 1 ? TIME_ENTITY[k]+ "s" : TIME_ENTITY[k]);</t>
-  </si>
-  <si>
     <t>sb.append(" ");</t>
   </si>
   <si>
     <t>return sb.toString();</t>
   </si>
   <si>
-    <t>16-12+2=6</t>
-  </si>
-  <si>
-    <t>5+1=6</t>
-  </si>
-  <si>
     <t>1 - 2(T)</t>
   </si>
   <si>
@@ -639,9 +630,6 @@
     <t>IllegalArgumentException</t>
   </si>
   <si>
-    <t>1, 2</t>
-  </si>
-  <si>
     <t>"1 day 2 hours 3 minutes"</t>
   </si>
   <si>
@@ -685,6 +673,60 @@
   </si>
   <si>
     <t>12% din metodele din clasa, 100% coverage a metodei</t>
+  </si>
+  <si>
+    <t>sb.append(time[k] &gt; 1 ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                TIME_ENTITY[k]+ "s" : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                TIME_ENTITY[k]);</t>
+  </si>
+  <si>
+    <t>13.</t>
+  </si>
+  <si>
+    <t>14.</t>
+  </si>
+  <si>
+    <t>15.</t>
+  </si>
+  <si>
+    <t>16.</t>
+  </si>
+  <si>
+    <t>21-16+2=7</t>
+  </si>
+  <si>
+    <t>6+1=6</t>
+  </si>
+  <si>
+    <t>1, 3, 4, 5, 7, 8, 9, 10, 11, 13, 14, 15, 16</t>
+  </si>
+  <si>
+    <t>1, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 14, 15, 16</t>
+  </si>
+  <si>
+    <t>1, 3, 4, 5, 6, 7, 9, 10, 11, 12, 14, 15, 16</t>
+  </si>
+  <si>
+    <t>1, 3, 4, 9, 10, 11, 12, 13, 14, 15, 16</t>
+  </si>
+  <si>
+    <t>1, 3, 4, 5, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16</t>
+  </si>
+  <si>
+    <t>1,2, 16</t>
+  </si>
+  <si>
+    <t>1, 2, 16</t>
+  </si>
+  <si>
+    <t>1, 3, 4, 5, 6, 7, 8, 9, 10, 11, 13, 14, 15, 16</t>
+  </si>
+  <si>
+    <t>F02_Cond06: time[k] &gt; 1</t>
   </si>
 </sst>
 </file>
@@ -1465,7 +1507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1574,6 +1616,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1584,20 +1641,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1607,8 +1673,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1622,17 +1691,134 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1646,147 +1832,9 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1795,6 +1843,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1817,23 +1871,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>99019</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>138111</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>20781</xdr:rowOff>
+      <xdr:rowOff>152847</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>135643</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>138841</xdr:rowOff>
+      <xdr:colOff>289746</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>81237</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{362F15B4-3B23-C637-1029-052F66827B11}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{193D1A42-2E46-A5C2-5E6C-F2C706A2F4D7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1849,8 +1903,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7708628" y="1492826"/>
-          <a:ext cx="5155879" cy="4558442"/>
+          <a:off x="7481886" y="1605410"/>
+          <a:ext cx="5523735" cy="4519440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1860,6 +1914,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2165,12 +2223,12 @@
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="12"/>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="50"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="55"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="40" t="s">
@@ -2294,10 +2352,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:R34"/>
+  <dimension ref="B1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2313,45 +2371,45 @@
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="12"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="50"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="55"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="58"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="66"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="49"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="33"/>
       <c r="E6" s="33"/>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="O6" s="48" t="s">
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="O6" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="49"/>
-      <c r="R6" s="49"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
     </row>
     <row r="8" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B8" s="34" t="s">
@@ -2365,13 +2423,13 @@
       <c r="G8" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="O8" s="55" t="s">
+      <c r="O8" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="P8" s="55"/>
-      <c r="Q8" s="55"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
       <c r="R8" s="41">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2382,13 +2440,13 @@
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="G9" s="39"/>
-      <c r="O9" s="55" t="s">
+      <c r="O9" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="60"/>
       <c r="R9" s="41" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2398,15 +2456,15 @@
       <c r="C10" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="O10" s="55" t="s">
+      <c r="O10" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="P10" s="55" t="s">
+      <c r="P10" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="Q10" s="55"/>
+      <c r="Q10" s="60"/>
       <c r="R10" s="41" t="s">
-        <v>112</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -2418,7 +2476,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="58" t="s">
         <v>79</v>
       </c>
       <c r="C12" s="44" t="s">
@@ -2426,121 +2484,121 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="52"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="O13" s="48" t="s">
+      <c r="O13" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="P13" s="49"/>
-      <c r="Q13" s="49"/>
-      <c r="R13" s="49"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="54"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="52"/>
+      <c r="B14" s="63"/>
       <c r="C14" s="44" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="52"/>
+      <c r="B15" s="63"/>
       <c r="C15" s="44" t="s">
         <v>98</v>
       </c>
       <c r="O15" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="P15" s="59" t="s">
+      <c r="P15" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="59"/>
-    </row>
-    <row r="16" spans="2:18" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="52"/>
+      <c r="Q15" s="61"/>
+      <c r="R15" s="61"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="63"/>
       <c r="C16" s="44" t="s">
         <v>99</v>
       </c>
       <c r="O16" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="P16" s="54" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q16" s="54"/>
-      <c r="R16" s="54"/>
+      <c r="P16" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q16" s="62"/>
+      <c r="R16" s="62"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="52"/>
+      <c r="B17" s="63"/>
       <c r="C17" s="44"/>
       <c r="O17" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="P17" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q17" s="54"/>
-      <c r="R17" s="54"/>
+      <c r="P17" s="62" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q17" s="62"/>
+      <c r="R17" s="62"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="52"/>
+      <c r="B18" s="63"/>
       <c r="C18" s="44" t="s">
         <v>100</v>
       </c>
       <c r="O18" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="P18" s="54" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="54"/>
+      <c r="P18" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q18" s="62"/>
+      <c r="R18" s="62"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="52"/>
+      <c r="B19" s="63"/>
       <c r="C19" s="44" t="s">
         <v>101</v>
       </c>
       <c r="O19" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="P19" s="54" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q19" s="54"/>
-      <c r="R19" s="54"/>
+      <c r="P19" s="62" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q19" s="62"/>
+      <c r="R19" s="62"/>
     </row>
     <row r="20" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B20" s="53"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="45" t="s">
         <v>102</v>
       </c>
       <c r="O20" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="P20" s="54" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q20" s="54"/>
-      <c r="R20" s="54"/>
+      <c r="P20" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q20" s="62"/>
+      <c r="R20" s="62"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="58" t="s">
         <v>80</v>
       </c>
       <c r="C21" s="44"/>
       <c r="O21" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="P21" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q21" s="54"/>
-      <c r="R21" s="54"/>
+      <c r="P21" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q21" s="62"/>
+      <c r="R21" s="62"/>
     </row>
     <row r="22" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B22" s="53"/>
+      <c r="B22" s="59"/>
       <c r="C22" s="45" t="s">
         <v>103</v>
       </c>
@@ -2570,7 +2628,7 @@
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="58" t="s">
         <v>87</v>
       </c>
       <c r="C26" s="44" t="s">
@@ -2578,7 +2636,7 @@
       </c>
     </row>
     <row r="27" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B27" s="53"/>
+      <c r="B27" s="59"/>
       <c r="C27" s="45" t="s">
         <v>85</v>
       </c>
@@ -2591,70 +2649,90 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B29" s="51" t="s">
+    <row r="29" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B29" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="44" t="s">
+      <c r="C29" s="43" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30" s="52"/>
-      <c r="C30" s="44" t="s">
+    <row r="30" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B30" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B31" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B32" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32" s="43" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" s="56" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="44" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B31" s="52"/>
-      <c r="C31" s="44" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B32" s="53"/>
-      <c r="C32" s="45" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B33" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" s="45" t="s">
-        <v>110</v>
-      </c>
-    </row>
     <row r="34" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B34" s="46" t="s">
-        <v>91</v>
-      </c>
+      <c r="B34" s="57"/>
       <c r="C34" s="45" t="s">
         <v>85</v>
       </c>
     </row>
+    <row r="35" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B35" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" s="45" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B36" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="C36" s="45" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="O13:R13"/>
+    <mergeCell ref="B12:B20"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="G6:M6"/>
     <mergeCell ref="O6:R6"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="O13:R13"/>
-    <mergeCell ref="B12:B20"/>
+    <mergeCell ref="B33:B34"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B29:B32"/>
     <mergeCell ref="O10:Q10"/>
     <mergeCell ref="P15:R15"/>
     <mergeCell ref="P17:R17"/>
     <mergeCell ref="P19:R19"/>
     <mergeCell ref="P20:R20"/>
     <mergeCell ref="P21:R21"/>
+    <mergeCell ref="P18:R18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2667,10 +2745,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:Z20"/>
+  <dimension ref="B1:AB20"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="74" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="74" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2687,175 +2765,185 @@
     <col min="11" max="11" width="6.1015625" customWidth="1"/>
     <col min="12" max="12" width="6.41796875" customWidth="1"/>
     <col min="13" max="13" width="17.734375" customWidth="1"/>
-    <col min="15" max="15" width="11.7890625" customWidth="1"/>
-    <col min="16" max="16" width="8.7890625" customWidth="1"/>
-    <col min="17" max="17" width="8.89453125" customWidth="1"/>
-    <col min="21" max="21" width="9.1015625" customWidth="1"/>
-    <col min="22" max="22" width="2.20703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="2.1015625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="2.1015625" customWidth="1"/>
-    <col min="26" max="26" width="3.5234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.15625" customWidth="1"/>
+    <col min="15" max="15" width="9.5234375" customWidth="1"/>
+    <col min="17" max="17" width="11.7890625" customWidth="1"/>
+    <col min="18" max="18" width="8.7890625" customWidth="1"/>
+    <col min="19" max="19" width="8.89453125" customWidth="1"/>
+    <col min="23" max="23" width="9.1015625" customWidth="1"/>
+    <col min="24" max="24" width="2.20703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="2.1015625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.1015625" customWidth="1"/>
+    <col min="28" max="28" width="3.5234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:28" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="12"/>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="50"/>
-    </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="64" t="s">
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="55"/>
+    </row>
+    <row r="3" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="58"/>
-    </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="66"/>
+    </row>
+    <row r="5" spans="2:28" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="11"/>
     </row>
-    <row r="6" spans="2:26" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="65" t="s">
+    <row r="6" spans="2:28" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="C6" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="66" t="s">
+      <c r="D6" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="108" t="s">
+      <c r="E6" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="109"/>
-      <c r="K6" s="109"/>
-      <c r="L6" s="109"/>
-      <c r="M6" s="109"/>
-      <c r="N6" s="109"/>
-      <c r="O6" s="109"/>
-      <c r="P6" s="109"/>
-      <c r="Q6" s="109"/>
-      <c r="R6" s="109"/>
-      <c r="S6" s="109"/>
-      <c r="T6" s="109"/>
-      <c r="U6" s="109"/>
-      <c r="V6" s="109"/>
-      <c r="W6" s="109"/>
-      <c r="X6" s="109"/>
-      <c r="Y6" s="109"/>
-      <c r="Z6" s="110"/>
-    </row>
-    <row r="7" spans="2:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="61" t="s">
+      <c r="F6" s="77"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="77"/>
+      <c r="P6" s="77"/>
+      <c r="Q6" s="77"/>
+      <c r="R6" s="77"/>
+      <c r="S6" s="77"/>
+      <c r="T6" s="77"/>
+      <c r="U6" s="77"/>
+      <c r="V6" s="77"/>
+      <c r="W6" s="77"/>
+      <c r="X6" s="77"/>
+      <c r="Y6" s="77"/>
+      <c r="Z6" s="77"/>
+      <c r="AA6" s="77"/>
+      <c r="AB6" s="78"/>
+    </row>
+    <row r="7" spans="2:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
-      <c r="O7" s="60"/>
-      <c r="P7" s="62" t="s">
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="69"/>
+      <c r="M7" s="69"/>
+      <c r="N7" s="69"/>
+      <c r="O7" s="69"/>
+      <c r="P7" s="69"/>
+      <c r="Q7" s="69"/>
+      <c r="R7" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="62"/>
-      <c r="S7" s="62"/>
-      <c r="T7" s="62"/>
-      <c r="U7" s="62"/>
-      <c r="V7" s="105" t="s">
+      <c r="S7" s="71"/>
+      <c r="T7" s="71"/>
+      <c r="U7" s="71"/>
+      <c r="V7" s="71"/>
+      <c r="W7" s="71"/>
+      <c r="X7" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="W7" s="106"/>
-      <c r="X7" s="106"/>
-      <c r="Y7" s="106"/>
-      <c r="Z7" s="107"/>
-    </row>
-    <row r="8" spans="2:26" ht="101.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="65"/>
-      <c r="C8" s="66" t="s">
-        <v>129</v>
-      </c>
-      <c r="D8" s="66" t="s">
-        <v>137</v>
-      </c>
-      <c r="E8" s="61"/>
-      <c r="F8" s="60" t="s">
+      <c r="Y7" s="74"/>
+      <c r="Z7" s="74"/>
+      <c r="AA7" s="74"/>
+      <c r="AB7" s="75"/>
+    </row>
+    <row r="8" spans="2:28" ht="101.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="82"/>
+      <c r="C8" s="67" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="70"/>
+      <c r="F8" s="69" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69" t="s">
+        <v>115</v>
+      </c>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69" t="s">
+        <v>116</v>
+      </c>
+      <c r="K8" s="69"/>
+      <c r="L8" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60" t="s">
+      <c r="M8" s="69"/>
+      <c r="N8" s="124" t="s">
         <v>118</v>
       </c>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60" t="s">
-        <v>120</v>
-      </c>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60" t="s">
-        <v>121</v>
-      </c>
-      <c r="O8" s="60"/>
-      <c r="P8" s="62" t="s">
+      <c r="O8" s="125"/>
+      <c r="P8" s="69" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q8" s="69"/>
+      <c r="R8" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="Q8" s="62" t="s">
+      <c r="S8" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="R8" s="62" t="s">
+      <c r="T8" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="S8" s="62" t="s">
+      <c r="U8" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="T8" s="62" t="s">
+      <c r="V8" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="U8" s="62" t="s">
+      <c r="W8" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="V8" s="63">
+      <c r="X8" s="72">
         <v>0</v>
       </c>
-      <c r="W8" s="63">
+      <c r="Y8" s="72">
         <v>1</v>
       </c>
-      <c r="X8" s="63">
+      <c r="Z8" s="72">
         <v>2</v>
       </c>
-      <c r="Y8" s="111">
+      <c r="AA8" s="79">
         <v>3</v>
       </c>
-      <c r="Z8" s="63">
+      <c r="AB8" s="72">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:26" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="65"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="61"/>
+    <row r="9" spans="2:28" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="82"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="70"/>
       <c r="F9" s="13" t="s">
         <v>21</v>
       </c>
@@ -2886,66 +2974,76 @@
       <c r="O9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="P9" s="62"/>
-      <c r="Q9" s="62"/>
-      <c r="R9" s="62"/>
-      <c r="S9" s="62"/>
-      <c r="T9" s="62"/>
-      <c r="U9" s="62"/>
-      <c r="V9" s="63"/>
-      <c r="W9" s="63"/>
-      <c r="X9" s="63"/>
-      <c r="Y9" s="112"/>
-      <c r="Z9" s="63"/>
-    </row>
-    <row r="10" spans="2:26" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="P9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="R9" s="71"/>
+      <c r="S9" s="71"/>
+      <c r="T9" s="71"/>
+      <c r="U9" s="71"/>
+      <c r="V9" s="71"/>
+      <c r="W9" s="71"/>
+      <c r="X9" s="72"/>
+      <c r="Y9" s="72"/>
+      <c r="Z9" s="72"/>
+      <c r="AA9" s="80"/>
+      <c r="AB9" s="72"/>
+    </row>
+    <row r="10" spans="2:28" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="C10" s="113">
+        <v>133</v>
+      </c>
+      <c r="C10" s="48">
         <v>0</v>
       </c>
-      <c r="D10" s="113" t="s">
-        <v>138</v>
+      <c r="D10" s="48" t="s">
+        <v>135</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
       <c r="I10" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J10" s="17"/>
       <c r="K10" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L10" s="17"/>
       <c r="M10" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="N10" s="17"/>
       <c r="O10" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="P10" s="114"/>
-      <c r="Q10" s="114"/>
-      <c r="R10" s="114"/>
-      <c r="S10" s="114"/>
-      <c r="T10" s="114"/>
-      <c r="U10" s="114"/>
-      <c r="V10" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="W10" s="19"/>
-      <c r="X10" s="19"/>
-      <c r="Y10" s="115"/>
+        <v>119</v>
+      </c>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="R10" s="49"/>
+      <c r="S10" s="49"/>
+      <c r="T10" s="49"/>
+      <c r="U10" s="49"/>
+      <c r="V10" s="49"/>
+      <c r="W10" s="49"/>
+      <c r="X10" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y10" s="19"/>
       <c r="Z10" s="19"/>
-    </row>
-    <row r="11" spans="2:26" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA10" s="50"/>
+      <c r="AB10" s="19"/>
+    </row>
+    <row r="11" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="14" t="s">
         <v>42</v>
       </c>
@@ -2953,46 +3051,50 @@
         <v>86400</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>116</v>
+        <v>160</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
       <c r="K11" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M11" s="17"/>
       <c r="N11" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O11" s="17"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17" t="s">
+        <v>119</v>
+      </c>
       <c r="R11" s="18"/>
       <c r="S11" s="18"/>
       <c r="T11" s="18"/>
       <c r="U11" s="18"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="19" t="s">
-        <v>122</v>
-      </c>
+      <c r="V11" s="18"/>
+      <c r="W11" s="18"/>
       <c r="X11" s="19"/>
-      <c r="Y11" s="19"/>
+      <c r="Y11" s="19" t="s">
+        <v>119</v>
+      </c>
       <c r="Z11" s="19"/>
-    </row>
-    <row r="12" spans="2:26" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
+    </row>
+    <row r="12" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="14" t="s">
         <v>43</v>
       </c>
@@ -3000,407 +3102,440 @@
         <v>7200</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I12" s="17"/>
       <c r="J12" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="K12" s="17"/>
       <c r="L12" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M12" s="17"/>
       <c r="N12" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O12" s="17"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
+      <c r="P12" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q12" s="17"/>
       <c r="R12" s="18"/>
       <c r="S12" s="18"/>
       <c r="T12" s="18"/>
       <c r="U12" s="18"/>
-      <c r="V12" s="19"/>
-      <c r="W12" s="19" t="s">
+      <c r="V12" s="18"/>
+      <c r="W12" s="18"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="19"/>
+      <c r="AB12" s="19"/>
+    </row>
+    <row r="13" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="14" t="s">
         <v>122</v>
-      </c>
-      <c r="X12" s="19"/>
-      <c r="Y12" s="19"/>
-      <c r="Z12" s="19"/>
-    </row>
-    <row r="13" spans="2:26" ht="31.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="14" t="s">
-        <v>125</v>
       </c>
       <c r="C13" s="20">
         <v>180</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I13" s="17"/>
       <c r="J13" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="K13" s="17"/>
       <c r="L13" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M13" s="17"/>
       <c r="N13" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O13" s="17"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
+      <c r="P13" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q13" s="17"/>
       <c r="R13" s="18"/>
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
       <c r="U13" s="18"/>
-      <c r="V13" s="19"/>
-      <c r="W13" s="19" t="s">
-        <v>122</v>
-      </c>
+      <c r="V13" s="18"/>
+      <c r="W13" s="18"/>
       <c r="X13" s="19"/>
-      <c r="Y13" s="19"/>
+      <c r="Y13" s="19" t="s">
+        <v>119</v>
+      </c>
       <c r="Z13" s="19"/>
-    </row>
-    <row r="14" spans="2:26" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="19"/>
+    </row>
+    <row r="14" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="14" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C14" s="14">
         <v>45</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>132</v>
+        <v>162</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I14" s="17"/>
       <c r="J14" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
       <c r="M14" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O14" s="17"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
+      <c r="P14" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q14" s="17"/>
       <c r="R14" s="18"/>
       <c r="S14" s="18"/>
       <c r="T14" s="18"/>
       <c r="U14" s="18"/>
-      <c r="V14" s="19"/>
-      <c r="W14" s="19" t="s">
-        <v>122</v>
-      </c>
+      <c r="V14" s="18"/>
+      <c r="W14" s="18"/>
       <c r="X14" s="19"/>
-      <c r="Y14" s="19"/>
+      <c r="Y14" s="19" t="s">
+        <v>119</v>
+      </c>
       <c r="Z14" s="19"/>
-    </row>
-    <row r="15" spans="2:26" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="19"/>
+    </row>
+    <row r="15" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="14" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C15" s="14">
         <v>93723</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J15" s="17"/>
       <c r="K15" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L15" s="17"/>
       <c r="M15" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="N15" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O15" s="17"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
+      <c r="P15" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q15" s="17"/>
       <c r="R15" s="18"/>
       <c r="S15" s="18"/>
       <c r="T15" s="18"/>
       <c r="U15" s="18"/>
-      <c r="V15" s="19"/>
-      <c r="W15" s="19"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
       <c r="X15" s="19"/>
       <c r="Y15" s="19"/>
-      <c r="Z15" s="19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="2:26" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="19"/>
+      <c r="AB15" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C16" s="14">
         <v>93680</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>116</v>
+        <v>164</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
       <c r="K16" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M16" s="17"/>
       <c r="N16" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O16" s="17"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
+      <c r="P16" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q16" s="17"/>
       <c r="R16" s="18"/>
       <c r="S16" s="18"/>
       <c r="T16" s="18"/>
       <c r="U16" s="18"/>
-      <c r="V16" s="19"/>
-      <c r="W16" s="19"/>
+      <c r="V16" s="18"/>
+      <c r="W16" s="18"/>
       <c r="X16" s="19"/>
-      <c r="Y16" s="19" t="s">
-        <v>122</v>
-      </c>
+      <c r="Y16" s="19"/>
       <c r="Z16" s="19"/>
-    </row>
-    <row r="17" spans="2:26" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA16" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB16" s="19"/>
+    </row>
+    <row r="17" spans="2:28" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="14" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C17" s="14">
         <v>-100</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="E17" s="16">
-        <v>1.2</v>
+        <v>135</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>165</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
       <c r="I17" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J17" s="17"/>
       <c r="K17" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L17" s="17"/>
       <c r="M17" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="N17" s="17"/>
       <c r="O17" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
+        <v>119</v>
+      </c>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17" t="s">
+        <v>119</v>
+      </c>
       <c r="R17" s="18"/>
       <c r="S17" s="18"/>
       <c r="T17" s="18"/>
       <c r="U17" s="18"/>
-      <c r="V17" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="W17" s="19"/>
-      <c r="X17" s="19"/>
+      <c r="V17" s="18"/>
+      <c r="W17" s="18"/>
+      <c r="X17" s="19" t="s">
+        <v>119</v>
+      </c>
       <c r="Y17" s="19"/>
       <c r="Z17" s="19"/>
-    </row>
-    <row r="18" spans="2:26" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AA17" s="19"/>
+      <c r="AB17" s="19"/>
+    </row>
+    <row r="18" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C18" s="14">
         <v>86430</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J18" s="17"/>
       <c r="K18" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L18" s="17"/>
       <c r="M18" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="N18" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O18" s="17"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
+      <c r="P18" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q18" s="17"/>
       <c r="R18" s="18"/>
       <c r="S18" s="18"/>
       <c r="T18" s="18"/>
       <c r="U18" s="18"/>
-      <c r="V18" s="19"/>
-      <c r="W18" s="19"/>
+      <c r="V18" s="18"/>
+      <c r="W18" s="18"/>
       <c r="X18" s="19"/>
       <c r="Y18" s="19"/>
-      <c r="Z18" s="19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="19" spans="2:26" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="Z18" s="19"/>
+      <c r="AA18" s="19"/>
+      <c r="AB18" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="14" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C19" s="14">
         <v>3660</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>124</v>
+        <v>167</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I19" s="17"/>
       <c r="J19" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="K19" s="17"/>
       <c r="L19" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M19" s="17"/>
       <c r="N19" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O19" s="17"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17" t="s">
+        <v>119</v>
+      </c>
       <c r="R19" s="18"/>
       <c r="S19" s="18"/>
       <c r="T19" s="18"/>
       <c r="U19" s="18"/>
-      <c r="V19" s="19"/>
-      <c r="W19" s="19"/>
-      <c r="X19" s="19" t="s">
-        <v>122</v>
-      </c>
+      <c r="V19" s="18"/>
+      <c r="W19" s="18"/>
+      <c r="X19" s="19"/>
       <c r="Y19" s="19"/>
-      <c r="Z19" s="19"/>
-    </row>
-    <row r="20" spans="2:26" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="Z19" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA19" s="19"/>
+      <c r="AB19" s="19"/>
+    </row>
+    <row r="20" spans="2:28" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="V7:Z7"/>
-    <mergeCell ref="E6:Z6"/>
-    <mergeCell ref="Y8:Y9"/>
+  <mergeCells count="29">
+    <mergeCell ref="X7:AB7"/>
+    <mergeCell ref="E6:AB6"/>
+    <mergeCell ref="AA8:AA9"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="W8:W9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="W8:W9"/>
+    <mergeCell ref="Y8:Y9"/>
+    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="X8:X9"/>
-    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
     <mergeCell ref="T8:T9"/>
-    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:Q7"/>
+    <mergeCell ref="R7:W7"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="C8:C9"/>
     <mergeCell ref="N8:O8"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:O7"/>
-    <mergeCell ref="P7:U7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3415,7 +3550,7 @@
   <dimension ref="B1:N21"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3435,63 +3570,63 @@
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="12"/>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="50"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="55"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="103" t="s">
+      <c r="D4" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="95" t="s">
+      <c r="E4" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="95" t="s">
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="96"/>
+      <c r="L4" s="106"/>
     </row>
     <row r="5" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B5" s="94"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="104"/>
-      <c r="E5" s="97" t="s">
+      <c r="B5" s="104"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="118"/>
-      <c r="I5" s="118"/>
-      <c r="J5" s="98"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114"/>
+      <c r="I5" s="114"/>
+      <c r="J5" s="115"/>
       <c r="K5" s="2" t="s">
         <v>4</v>
       </c>
@@ -3503,222 +3638,232 @@
       <c r="B6" s="23">
         <v>9</v>
       </c>
-      <c r="C6" s="99" t="s">
+      <c r="C6" s="107" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E6" s="119">
+        <v>133</v>
+      </c>
+      <c r="E6" s="121">
         <v>0</v>
       </c>
-      <c r="F6" s="120"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="120"/>
-      <c r="I6" s="120"/>
-      <c r="J6" s="121"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="123"/>
       <c r="K6" s="24" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="L6" s="23" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="23">
         <v>10</v>
       </c>
-      <c r="C7" s="99"/>
+      <c r="C7" s="107"/>
       <c r="D7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="95">
+      <c r="E7" s="105">
         <v>86400</v>
       </c>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="96"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="106"/>
       <c r="K7" s="23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="23">
         <v>11</v>
       </c>
-      <c r="C8" s="99"/>
+      <c r="C8" s="107"/>
       <c r="D8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="95">
+      <c r="E8" s="105">
         <v>7200</v>
       </c>
-      <c r="F8" s="101"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="96"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="106"/>
       <c r="K8" s="23" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="23">
         <v>12</v>
       </c>
-      <c r="C9" s="99"/>
+      <c r="C9" s="107"/>
       <c r="D9" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="105">
+        <v>180</v>
+      </c>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="106"/>
+      <c r="K9" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="23">
+        <v>13</v>
+      </c>
+      <c r="C10" s="107"/>
+      <c r="D10" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="105">
+        <v>45</v>
+      </c>
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="106"/>
+      <c r="K10" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="L10" s="51" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="23">
+        <v>14</v>
+      </c>
+      <c r="C11" s="107"/>
+      <c r="D11" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="105">
+        <v>93723</v>
+      </c>
+      <c r="F11" s="109"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="106"/>
+      <c r="K11" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="L11" s="51" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="23">
+        <v>15</v>
+      </c>
+      <c r="C12" s="107"/>
+      <c r="D12" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" s="105">
+        <v>86430</v>
+      </c>
+      <c r="F12" s="109"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="109"/>
+      <c r="I12" s="109"/>
+      <c r="J12" s="106"/>
+      <c r="K12" s="51" t="s">
+        <v>148</v>
+      </c>
+      <c r="L12" s="51" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="23">
+        <v>16</v>
+      </c>
+      <c r="C13" s="107"/>
+      <c r="D13" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" s="105">
+        <v>3660</v>
+      </c>
+      <c r="F13" s="109"/>
+      <c r="G13" s="109"/>
+      <c r="H13" s="109"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="106"/>
+      <c r="K13" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="L13" s="51" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="23">
+        <v>17</v>
+      </c>
+      <c r="C14" s="107"/>
+      <c r="D14" s="52" t="s">
         <v>125</v>
       </c>
-      <c r="E9" s="95">
-        <v>180</v>
-      </c>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="96"/>
-      <c r="K9" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="L9" s="23" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="116"/>
-      <c r="C10" s="99"/>
-      <c r="D10" s="117" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" s="95">
-        <v>45</v>
-      </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="96"/>
-      <c r="K10" s="116" t="s">
-        <v>131</v>
-      </c>
-      <c r="L10" s="116" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="116"/>
-      <c r="C11" s="99"/>
-      <c r="D11" s="117" t="s">
-        <v>127</v>
-      </c>
-      <c r="E11" s="95">
-        <v>93723</v>
-      </c>
-      <c r="F11" s="101"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="101"/>
-      <c r="I11" s="101"/>
-      <c r="J11" s="96"/>
-      <c r="K11" s="116" t="s">
-        <v>133</v>
-      </c>
-      <c r="L11" s="116" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="116"/>
-      <c r="C12" s="99"/>
-      <c r="D12" s="117" t="s">
-        <v>142</v>
-      </c>
-      <c r="E12" s="95">
-        <v>86430</v>
-      </c>
-      <c r="F12" s="101"/>
-      <c r="G12" s="101"/>
-      <c r="H12" s="101"/>
-      <c r="I12" s="101"/>
-      <c r="J12" s="96"/>
-      <c r="K12" s="116" t="s">
-        <v>152</v>
-      </c>
-      <c r="L12" s="116" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="116"/>
-      <c r="C13" s="99"/>
-      <c r="D13" s="117" t="s">
-        <v>143</v>
-      </c>
-      <c r="E13" s="95">
-        <v>3660</v>
-      </c>
-      <c r="F13" s="101"/>
-      <c r="G13" s="101"/>
-      <c r="H13" s="101"/>
-      <c r="I13" s="101"/>
-      <c r="J13" s="96"/>
-      <c r="K13" s="116" t="s">
+      <c r="E14" s="105">
+        <v>93680</v>
+      </c>
+      <c r="F14" s="109"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="109"/>
+      <c r="I14" s="109"/>
+      <c r="J14" s="106"/>
+      <c r="K14" s="51" t="s">
+        <v>136</v>
+      </c>
+      <c r="L14" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B15" s="23">
+        <v>18</v>
+      </c>
+      <c r="C15" s="108"/>
+      <c r="D15" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" s="105">
+        <v>-100</v>
+      </c>
+      <c r="F15" s="109"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="109"/>
+      <c r="J15" s="106"/>
+      <c r="K15" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="L13" s="116" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="116"/>
-      <c r="C14" s="99"/>
-      <c r="D14" s="117" t="s">
-        <v>128</v>
-      </c>
-      <c r="E14" s="95">
-        <v>93680</v>
-      </c>
-      <c r="F14" s="101"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="101"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="96"/>
-      <c r="K14" s="116" t="s">
-        <v>140</v>
-      </c>
-      <c r="L14" s="116" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B15" s="2">
-        <v>13</v>
-      </c>
-      <c r="C15" s="100"/>
-      <c r="D15" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E15" s="95">
-        <v>-100</v>
-      </c>
-      <c r="F15" s="101"/>
-      <c r="G15" s="101"/>
-      <c r="H15" s="101"/>
-      <c r="I15" s="101"/>
-      <c r="J15" s="96"/>
-      <c r="K15" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="L15" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
@@ -3741,83 +3886,83 @@
       <c r="K17" s="25"/>
     </row>
     <row r="18" spans="2:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="116" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="70" t="s">
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="118" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="71"/>
-      <c r="H18" s="68" t="s">
+      <c r="G18" s="119"/>
+      <c r="H18" s="116" t="s">
         <v>59</v>
       </c>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="86"/>
-      <c r="M18" s="90" t="s">
+      <c r="I18" s="117"/>
+      <c r="J18" s="117"/>
+      <c r="K18" s="117"/>
+      <c r="L18" s="120"/>
+      <c r="M18" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="N18" s="91"/>
+      <c r="N18" s="101"/>
     </row>
     <row r="19" spans="2:14" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="77" t="s">
+      <c r="C19" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="77" t="s">
+      <c r="D19" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="83" t="s">
+      <c r="E19" s="87" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="74" t="s">
+      <c r="F19" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="72" t="s">
+      <c r="G19" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="75" t="s">
+      <c r="H19" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="I19" s="77" t="s">
+      <c r="I19" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="J19" s="77" t="s">
+      <c r="J19" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="K19" s="79" t="s">
+      <c r="K19" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="L19" s="87" t="s">
+      <c r="L19" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="M19" s="89" t="s">
+      <c r="M19" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="N19" s="73" t="s">
+      <c r="N19" s="92" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="82"/>
-      <c r="C20" s="78"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="84"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="72"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="80"/>
-      <c r="L20" s="88"/>
-      <c r="M20" s="81"/>
-      <c r="N20" s="74"/>
+      <c r="B20" s="84"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="91"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="86"/>
+      <c r="J20" s="86"/>
+      <c r="K20" s="96"/>
+      <c r="L20" s="98"/>
+      <c r="M20" s="83"/>
+      <c r="N20" s="89"/>
     </row>
     <row r="21" spans="2:14" ht="41.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="29">
@@ -3831,7 +3976,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F21" s="28">
         <v>2</v>
@@ -3840,7 +3985,7 @@
         <v>2</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I21" s="29">
         <v>9</v>
@@ -3852,10 +3997,10 @@
         <v>2</v>
       </c>
       <c r="L21" s="31" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="N21" s="32">
         <f>C21</f>
@@ -3864,16 +4009,13 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E14:J14"/>
     <mergeCell ref="E15:J15"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E13:J13"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:L3"/>
@@ -3886,20 +4028,23 @@
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="N19:N20"/>
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="I19:I20"/>
     <mergeCell ref="K19:K20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated paths in excel
</commit_message>
<xml_diff>
--- a/Lab03/Docs/Lab03_WBT_TCs_Form.xlsx
+++ b/Lab03/Docs/Lab03_WBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="554" documentId="11_6DFBBE858289C8C7F32634D05F6B97BC65B49737" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D177F855-427C-4630-8EE6-F559F7A9FCC9}"/>
+  <xr:revisionPtr revIDLastSave="659" documentId="11_6DFBBE858289C8C7F32634D05F6B97BC65B49737" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48A9B67F-694D-457B-8717-A8D6052B4462}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="178">
   <si>
     <t>Informaţiile vor fi preluate din fişiere text.</t>
   </si>
@@ -51,13 +51,7 @@
     <t>actual result</t>
   </si>
   <si>
-    <t>..</t>
-  </si>
-  <si>
     <t>Final        TC No.</t>
-  </si>
-  <si>
-    <t>...</t>
   </si>
   <si>
     <t>Req. ID</t>
@@ -552,18 +546,9 @@
     <t>return sb.toString();</t>
   </si>
   <si>
-    <t>1 - 2(T)</t>
-  </si>
-  <si>
-    <t>1 - 2(F) - 3 - 4(T) - 5(T) - 6 - 7(T) - 8 - 4 - 9(T) - 10 - 9(F) - 11 - 12</t>
-  </si>
-  <si>
     <t>"1 day"</t>
   </si>
   <si>
-    <t>1, 3, 4, 5, 7, 8, 9, 10, 11, 12</t>
-  </si>
-  <si>
     <t>F02_Cond01: input &lt;= 0</t>
   </si>
   <si>
@@ -585,9 +570,6 @@
     <t>"2 hours"</t>
   </si>
   <si>
-    <t>1, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12</t>
-  </si>
-  <si>
     <t>F02_TC03</t>
   </si>
   <si>
@@ -609,15 +591,9 @@
     <t>"45 seconds"</t>
   </si>
   <si>
-    <t>1, 3, 4, 5, 6, 7, 9, 10, 11, 12</t>
-  </si>
-  <si>
     <t>"1 day 2 hours 3 minutes 43 seconds"</t>
   </si>
   <si>
-    <t>1, 3, 4, 9, 10, 11, 12</t>
-  </si>
-  <si>
     <t>"1 hour 1 minute"</t>
   </si>
   <si>
@@ -727,6 +703,57 @@
   </si>
   <si>
     <t>F02_Cond06: time[k] &gt; 1</t>
+  </si>
+  <si>
+    <t>F02_P04</t>
+  </si>
+  <si>
+    <t>F02_P05</t>
+  </si>
+  <si>
+    <t>F02_P06</t>
+  </si>
+  <si>
+    <t>F02_P07</t>
+  </si>
+  <si>
+    <t>1(F) - 3 - 4(T) - 5(F) - 7(T) - 8 - 9(T) - 10 - 11(F) - 13 - 14 - 9(F) - 15 - 16</t>
+  </si>
+  <si>
+    <t>F02_P08</t>
+  </si>
+  <si>
+    <t>1(F) - 3 - 4(T) - 5(T) - 6 - 7(T) - 8 - 4(T) - 5(T) - 6 - 7(F) - 4(T) - 5(T) - 6 - 7(F) - 4(F) - 9(T) - 10 - 11(T) - 12 - 14 - 9(F) - 15 - 16</t>
+  </si>
+  <si>
+    <t>1(F) - 3 - 4(T) - 5(T) - 6 - 7(F) - 4(T) - 5(T) - 6 - 7(F) - 4(T) - 5(T) - 6 - 7(F) - 4(F) - 9(T) - 10 - 11(T) - 12 - 14 - 15 - 16</t>
+  </si>
+  <si>
+    <t>1(F) - 3 - 4(T) - 5(F) - 7(F) - 4(F) - 9(T) - 10 - 11(F) - 13 - 14 - 9(T) - 10 - 11(T) - 12 - 14 - 9(T) - 10 - 11(T) - 12 - 14  - 9(T) - 10 - 11(T) - 12 - 14 - 9(F) - 15 - 16</t>
+  </si>
+  <si>
+    <t>1(F) - 3 - 4(T) - 5(F) - 7(F) - 4(F) - 9(T) - 10 - 11(F) - 13 - 14 - 9(T) - 10 - 11(T) - 12 - 14 - 9(T) - 10 - 11(T) - 12 - 14 - 9(F) - 15 - 16</t>
+  </si>
+  <si>
+    <t>1(F) - 3 - 4(T) - 5(F) - 7(F) - 4(F) - 9(T) - 10 - 11(F) - 13 - 14 - 9(T) - 10 - 11(F) - 13 - 14 - 9(T) - 10 - 11(F) - 13 - 14  - 9(T) - 10 - 11(T) - 12 - 14 - 9(F) - 15 - 16</t>
+  </si>
+  <si>
+    <t>1(F) - 3 - 4(T) - 5(F) - 7(F) - 4(T) - 5(T) - 6 - 7(T) - 8 - 4(F) - 9(T) - 10 - 11(F) - 13 - 14 - 9(T) - 10 - 11(F) - 13 - 14  - 9(F) - 15 - 16</t>
+  </si>
+  <si>
+    <t>F02_P09</t>
+  </si>
+  <si>
+    <t>1(F) - 3 - 4(T) - 5(F) - 7(F) - 4(T) - 5(T) - 6 - 7(F) - 4(F) - 9(T) - 10 - 11(F) - 13 - 14 - 9(T) - 10 - 11(F) - 13 - 14 - 9(T) - 10 - 11(T) - 12 - 14  - 9(F) - 15 - 16</t>
+  </si>
+  <si>
+    <t>F02_P10</t>
+  </si>
+  <si>
+    <t>1(F) - 3 - 4(T) - 5(T) - 6 - 7(T) - 8 - 4(T) - 5(F) - 7(T) - 8 - 4(F) - 9(T) - 10 - 11(T) - 12 - 14 - 9(F) - 15 - 16</t>
+  </si>
+  <si>
+    <t>1(T) - 2 - 16</t>
   </si>
 </sst>
 </file>
@@ -1507,7 +1534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1631,6 +1658,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1640,38 +1670,68 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1679,46 +1739,130 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1727,127 +1871,37 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1880,7 +1934,7 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>289746</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>81237</xdr:rowOff>
+      <xdr:rowOff>105049</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2223,34 +2277,34 @@
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="12"/>
-      <c r="D1" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="55"/>
+      <c r="D1" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="56"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N5" s="36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O5" s="36"/>
       <c r="P5" s="36"/>
@@ -2261,10 +2315,10 @@
       </c>
       <c r="N6" s="29"/>
       <c r="O6" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P6" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.55000000000000004">
@@ -2273,13 +2327,13 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="N7" s="29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O7" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P7" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.55000000000000004">
@@ -2288,30 +2342,30 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="N8" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="O8" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P8" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="N9" s="29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O9" s="29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P9" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.55000000000000004">
@@ -2321,7 +2375,7 @@
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2352,10 +2406,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:R36"/>
+  <dimension ref="B1:R43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17:R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2365,69 +2419,69 @@
     <col min="4" max="4" width="3.62890625" customWidth="1"/>
     <col min="5" max="5" width="4.89453125" customWidth="1"/>
     <col min="6" max="6" width="3.5234375" customWidth="1"/>
-    <col min="15" max="15" width="10.68359375" customWidth="1"/>
-    <col min="18" max="18" width="30.89453125" customWidth="1"/>
+    <col min="15" max="15" width="8.41796875" customWidth="1"/>
+    <col min="18" max="18" width="65.62890625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="12"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="56"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="66"/>
+      <c r="B3" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="54"/>
+      <c r="B6" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="55"/>
       <c r="D6" s="33"/>
       <c r="E6" s="33"/>
-      <c r="G6" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="O6" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="P6" s="54"/>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="54"/>
+      <c r="G6" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="55"/>
+      <c r="O6" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="P6" s="55"/>
+      <c r="Q6" s="55"/>
+      <c r="R6" s="55"/>
     </row>
     <row r="8" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B8" s="34" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="35"/>
       <c r="E8" s="35"/>
       <c r="G8" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="O8" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="60"/>
+        <v>66</v>
+      </c>
+      <c r="O8" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="P8" s="57"/>
+      <c r="Q8" s="57"/>
       <c r="R8" s="41">
         <v>7</v>
       </c>
@@ -2435,304 +2489,383 @@
     <row r="9" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B9" s="42"/>
       <c r="C9" s="43" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="G9" s="39"/>
-      <c r="O9" s="60" t="s">
-        <v>29</v>
-      </c>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="60"/>
+      <c r="O9" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" s="57"/>
+      <c r="Q9" s="57"/>
       <c r="R9" s="41" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B10" s="46" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="O10" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q10" s="60"/>
+        <v>91</v>
+      </c>
+      <c r="O10" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="57"/>
       <c r="R10" s="41" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B11" s="46" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C11" s="45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="60"/>
+      <c r="C13" s="44" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="58" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="44" t="s">
+      <c r="O13" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="P13" s="55"/>
+      <c r="Q13" s="55"/>
+      <c r="R13" s="55"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="60"/>
+      <c r="C14" s="44" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="63"/>
-      <c r="C13" s="44" t="s">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="60"/>
+      <c r="C15" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="O13" s="53" t="s">
-        <v>41</v>
-      </c>
-      <c r="P13" s="54"/>
-      <c r="Q13" s="54"/>
-      <c r="R13" s="54"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="63"/>
-      <c r="C14" s="44" t="s">
+      <c r="O15" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="P15" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q15" s="67"/>
+      <c r="R15" s="67"/>
+    </row>
+    <row r="16" spans="2:18" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="60"/>
+      <c r="C16" s="44" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="63"/>
-      <c r="C15" s="44" t="s">
-        <v>98</v>
-      </c>
-      <c r="O15" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="P15" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q15" s="61"/>
-      <c r="R15" s="61"/>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="63"/>
-      <c r="C16" s="44" t="s">
-        <v>99</v>
-      </c>
       <c r="O16" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="P16" s="62" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q16" s="62"/>
-      <c r="R16" s="62"/>
+        <v>42</v>
+      </c>
+      <c r="P16" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q16" s="58"/>
+      <c r="R16" s="58"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="63"/>
+      <c r="B17" s="60"/>
       <c r="C17" s="44"/>
       <c r="O17" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="P17" s="130" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q17" s="131"/>
+      <c r="R17" s="132"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="60"/>
+      <c r="C18" s="44"/>
+      <c r="O18" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="P17" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q17" s="62"/>
-      <c r="R17" s="62"/>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="63"/>
-      <c r="C18" s="44" t="s">
+      <c r="P18" s="130" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q18" s="131"/>
+      <c r="R18" s="132"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="60"/>
+      <c r="C19" s="44"/>
+      <c r="O19" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="P19" s="58" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q19" s="58"/>
+      <c r="R19" s="58"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="60"/>
+      <c r="C20" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="O20" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="P20" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q20" s="58"/>
+      <c r="R20" s="58"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="60"/>
+      <c r="C21" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="O21" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="P21" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q21" s="58"/>
+      <c r="R21" s="58"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="60"/>
+      <c r="C22" s="44"/>
+      <c r="O22" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="P22" s="130" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q22" s="131"/>
+      <c r="R22" s="132"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" s="60"/>
+      <c r="C23" s="44"/>
+      <c r="O23" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="P23" s="130" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q23" s="131"/>
+      <c r="R23" s="132"/>
+    </row>
+    <row r="24" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B24" s="61"/>
+      <c r="C24" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="O18" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="P18" s="62" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q18" s="62"/>
-      <c r="R18" s="62"/>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="63"/>
-      <c r="C19" s="44" t="s">
+      <c r="O24" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="P24" s="58" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q24" s="58"/>
+      <c r="R24" s="58"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" s="53"/>
+      <c r="C25" s="44"/>
+      <c r="O25" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="P25" s="130" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q25" s="131"/>
+      <c r="R25" s="132"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26" s="53"/>
+      <c r="C26" s="44"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="127"/>
+      <c r="Q26" s="128"/>
+      <c r="R26" s="129"/>
+    </row>
+    <row r="27" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B27" s="53"/>
+      <c r="C27" s="44"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="127"/>
+      <c r="Q27" s="128"/>
+      <c r="R27" s="129"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="44"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="58"/>
+      <c r="Q28" s="58"/>
+      <c r="R28" s="58"/>
+    </row>
+    <row r="29" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B29" s="61"/>
+      <c r="C29" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="O19" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="P19" s="62" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q19" s="62"/>
-      <c r="R19" s="62"/>
-    </row>
-    <row r="20" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B20" s="59"/>
-      <c r="C20" s="45" t="s">
+    </row>
+    <row r="30" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B30" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="O20" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="P20" s="62" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q20" s="62"/>
-      <c r="R20" s="62"/>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="58" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="44"/>
-      <c r="O21" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="P21" s="62" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q21" s="62"/>
-      <c r="R21" s="62"/>
-    </row>
-    <row r="22" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B22" s="59"/>
-      <c r="C22" s="45" t="s">
+    </row>
+    <row r="31" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B31" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B32" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="45" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B23" s="46" t="s">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="45" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B24" s="46" t="s">
+    </row>
+    <row r="34" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B34" s="61"/>
+      <c r="C34" s="45" t="s">
         <v>83</v>
-      </c>
-      <c r="C24" s="45" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B25" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B26" s="58" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="44" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B27" s="59"/>
-      <c r="C27" s="45" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B28" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" s="45" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B29" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" s="43" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B30" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="43" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="31" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B31" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="C31" s="43" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="32" spans="2:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B32" s="42" t="s">
-        <v>154</v>
-      </c>
-      <c r="C32" s="43" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B33" s="56" t="s">
-        <v>155</v>
-      </c>
-      <c r="C33" s="44" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B34" s="57"/>
-      <c r="C34" s="45" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B35" s="46" t="s">
-        <v>156</v>
+        <v>86</v>
       </c>
       <c r="C35" s="45" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B36" s="46" t="s">
-        <v>157</v>
-      </c>
-      <c r="C36" s="45" t="s">
-        <v>85</v>
+      <c r="B36" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B37" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="43" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B38" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B39" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="C39" s="43" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" s="65" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" s="44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B41" s="66"/>
+      <c r="C41" s="45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B42" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B43" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="C43" s="45" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="27">
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="P22:R22"/>
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="P16:R16"/>
     <mergeCell ref="O13:R13"/>
-    <mergeCell ref="B12:B20"/>
+    <mergeCell ref="B12:B24"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="G6:M6"/>
     <mergeCell ref="O6:R6"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="P23:R23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2745,10 +2878,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:AB20"/>
+  <dimension ref="B1:AF20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="74" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView topLeftCell="A5" zoomScale="74" workbookViewId="0">
+      <selection activeCell="Z20" sqref="Z20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2770,518 +2903,572 @@
     <col min="17" max="17" width="11.7890625" customWidth="1"/>
     <col min="18" max="18" width="8.7890625" customWidth="1"/>
     <col min="19" max="19" width="8.89453125" customWidth="1"/>
-    <col min="23" max="23" width="9.1015625" customWidth="1"/>
-    <col min="24" max="24" width="2.20703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="2.1015625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.1015625" customWidth="1"/>
-    <col min="28" max="28" width="3.5234375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.1015625" customWidth="1"/>
+    <col min="28" max="28" width="2.20703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="2.1015625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="2.1015625" customWidth="1"/>
+    <col min="32" max="32" width="3.5234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:32" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="12"/>
-      <c r="D1" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="55"/>
-    </row>
-    <row r="3" spans="2:28" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="81" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="66"/>
-    </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="D1" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="56"/>
+    </row>
+    <row r="3" spans="2:32" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="76" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="64"/>
+    </row>
+    <row r="5" spans="2:32" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="11"/>
     </row>
-    <row r="6" spans="2:28" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="82" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="82" t="s">
+    <row r="6" spans="2:32" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="77" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="67" t="s">
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="72"/>
+      <c r="O6" s="72"/>
+      <c r="P6" s="72"/>
+      <c r="Q6" s="72"/>
+      <c r="R6" s="72"/>
+      <c r="S6" s="72"/>
+      <c r="T6" s="72"/>
+      <c r="U6" s="72"/>
+      <c r="V6" s="72"/>
+      <c r="W6" s="72"/>
+      <c r="X6" s="72"/>
+      <c r="Y6" s="72"/>
+      <c r="Z6" s="72"/>
+      <c r="AA6" s="72"/>
+      <c r="AB6" s="72"/>
+      <c r="AC6" s="72"/>
+      <c r="AD6" s="72"/>
+      <c r="AE6" s="72"/>
+      <c r="AF6" s="73"/>
+    </row>
+    <row r="7" spans="2:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="83" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="81"/>
+      <c r="R7" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="S7" s="80"/>
+      <c r="T7" s="80"/>
+      <c r="U7" s="80"/>
+      <c r="V7" s="80"/>
+      <c r="W7" s="80"/>
+      <c r="X7" s="80"/>
+      <c r="Y7" s="80"/>
+      <c r="Z7" s="80"/>
+      <c r="AA7" s="80"/>
+      <c r="AB7" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="76" t="s">
+      <c r="AC7" s="69"/>
+      <c r="AD7" s="69"/>
+      <c r="AE7" s="69"/>
+      <c r="AF7" s="70"/>
+    </row>
+    <row r="8" spans="2:32" ht="101.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="77"/>
+      <c r="C8" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="78" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="83"/>
+      <c r="F8" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81" t="s">
+        <v>111</v>
+      </c>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="M8" s="81"/>
+      <c r="N8" s="84" t="s">
+        <v>113</v>
+      </c>
+      <c r="O8" s="85"/>
+      <c r="P8" s="81" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q8" s="81"/>
+      <c r="R8" s="80" t="s">
+        <v>42</v>
+      </c>
+      <c r="S8" s="80" t="s">
+        <v>43</v>
+      </c>
+      <c r="T8" s="80" t="s">
+        <v>45</v>
+      </c>
+      <c r="U8" s="80" t="s">
+        <v>161</v>
+      </c>
+      <c r="V8" s="80" t="s">
+        <v>162</v>
+      </c>
+      <c r="W8" s="133" t="s">
+        <v>163</v>
+      </c>
+      <c r="X8" s="133" t="s">
+        <v>164</v>
+      </c>
+      <c r="Y8" s="133" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z8" s="133" t="s">
+        <v>173</v>
+      </c>
+      <c r="AA8" s="80" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB8" s="82">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="82">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="82">
+        <v>2</v>
+      </c>
+      <c r="AE8" s="74">
+        <v>3</v>
+      </c>
+      <c r="AF8" s="82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="77"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="77"/>
-      <c r="Q6" s="77"/>
-      <c r="R6" s="77"/>
-      <c r="S6" s="77"/>
-      <c r="T6" s="77"/>
-      <c r="U6" s="77"/>
-      <c r="V6" s="77"/>
-      <c r="W6" s="77"/>
-      <c r="X6" s="77"/>
-      <c r="Y6" s="77"/>
-      <c r="Z6" s="77"/>
-      <c r="AA6" s="77"/>
-      <c r="AB6" s="78"/>
-    </row>
-    <row r="7" spans="2:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="70" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="69" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="69"/>
-      <c r="R7" s="71" t="s">
-        <v>55</v>
-      </c>
-      <c r="S7" s="71"/>
-      <c r="T7" s="71"/>
-      <c r="U7" s="71"/>
-      <c r="V7" s="71"/>
-      <c r="W7" s="71"/>
-      <c r="X7" s="73" t="s">
+      <c r="G9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="Y7" s="74"/>
-      <c r="Z7" s="74"/>
-      <c r="AA7" s="74"/>
-      <c r="AB7" s="75"/>
-    </row>
-    <row r="8" spans="2:28" ht="101.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="82"/>
-      <c r="C8" s="67" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="67" t="s">
-        <v>134</v>
-      </c>
-      <c r="E8" s="70"/>
-      <c r="F8" s="69" t="s">
-        <v>114</v>
-      </c>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69" t="s">
-        <v>115</v>
-      </c>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69" t="s">
-        <v>116</v>
-      </c>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69" t="s">
-        <v>117</v>
-      </c>
-      <c r="M8" s="69"/>
-      <c r="N8" s="124" t="s">
-        <v>118</v>
-      </c>
-      <c r="O8" s="125"/>
-      <c r="P8" s="69" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="71" t="s">
-        <v>44</v>
-      </c>
-      <c r="S8" s="71" t="s">
-        <v>45</v>
-      </c>
-      <c r="T8" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="U8" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="V8" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="W8" s="71" t="s">
-        <v>46</v>
-      </c>
-      <c r="X8" s="72">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="72">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="72">
-        <v>2</v>
-      </c>
-      <c r="AA8" s="79">
-        <v>3</v>
-      </c>
-      <c r="AB8" s="72">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:28" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="82"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>22</v>
-      </c>
       <c r="H9" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O9" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P9" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q9" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="R9" s="71"/>
-      <c r="S9" s="71"/>
-      <c r="T9" s="71"/>
-      <c r="U9" s="71"/>
-      <c r="V9" s="71"/>
-      <c r="W9" s="71"/>
-      <c r="X9" s="72"/>
-      <c r="Y9" s="72"/>
-      <c r="Z9" s="72"/>
+        <v>20</v>
+      </c>
+      <c r="R9" s="80"/>
+      <c r="S9" s="80"/>
+      <c r="T9" s="80"/>
+      <c r="U9" s="80"/>
+      <c r="V9" s="80"/>
+      <c r="W9" s="134"/>
+      <c r="X9" s="134"/>
+      <c r="Y9" s="134"/>
+      <c r="Z9" s="134"/>
       <c r="AA9" s="80"/>
-      <c r="AB9" s="72"/>
-    </row>
-    <row r="10" spans="2:28" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB9" s="82"/>
+      <c r="AC9" s="82"/>
+      <c r="AD9" s="82"/>
+      <c r="AE9" s="75"/>
+      <c r="AF9" s="82"/>
+    </row>
+    <row r="10" spans="2:32" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="15" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C10" s="48">
         <v>0</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
       <c r="I10" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J10" s="17"/>
       <c r="K10" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L10" s="17"/>
       <c r="M10" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="N10" s="17"/>
       <c r="O10" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="P10" s="17"/>
       <c r="Q10" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="R10" s="49"/>
+        <v>114</v>
+      </c>
+      <c r="R10" s="49" t="s">
+        <v>114</v>
+      </c>
       <c r="S10" s="49"/>
       <c r="T10" s="49"/>
       <c r="U10" s="49"/>
       <c r="V10" s="49"/>
       <c r="W10" s="49"/>
-      <c r="X10" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y10" s="19"/>
-      <c r="Z10" s="19"/>
-      <c r="AA10" s="50"/>
-      <c r="AB10" s="19"/>
-    </row>
-    <row r="11" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="X10" s="49"/>
+      <c r="Y10" s="49"/>
+      <c r="Z10" s="49"/>
+      <c r="AA10" s="49"/>
+      <c r="AB10" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC10" s="19"/>
+      <c r="AD10" s="19"/>
+      <c r="AE10" s="50"/>
+      <c r="AF10" s="19"/>
+    </row>
+    <row r="11" spans="2:32" ht="31.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" s="14">
         <v>86400</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
       <c r="K11" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="M11" s="17"/>
       <c r="N11" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="O11" s="17"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
+      <c r="S11" s="18" t="s">
+        <v>114</v>
+      </c>
       <c r="T11" s="18"/>
       <c r="U11" s="18"/>
       <c r="V11" s="18"/>
       <c r="W11" s="18"/>
-      <c r="X11" s="19"/>
-      <c r="Y11" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z11" s="19"/>
-      <c r="AA11" s="19"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="18"/>
+      <c r="AA11" s="18"/>
       <c r="AB11" s="19"/>
-    </row>
-    <row r="12" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC11" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD11" s="19"/>
+      <c r="AE11" s="19"/>
+      <c r="AF11" s="19"/>
+    </row>
+    <row r="12" spans="2:32" ht="31.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" s="14">
         <v>7200</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I12" s="17"/>
       <c r="J12" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="K12" s="17"/>
       <c r="L12" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="M12" s="17"/>
       <c r="N12" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="O12" s="17"/>
       <c r="P12" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="Q12" s="17"/>
       <c r="R12" s="18"/>
       <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
+      <c r="T12" s="18" t="s">
+        <v>114</v>
+      </c>
       <c r="U12" s="18"/>
       <c r="V12" s="18"/>
       <c r="W12" s="18"/>
-      <c r="X12" s="19"/>
-      <c r="Y12" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z12" s="19"/>
-      <c r="AA12" s="19"/>
+      <c r="X12" s="18"/>
+      <c r="Y12" s="18"/>
+      <c r="Z12" s="18"/>
+      <c r="AA12" s="18"/>
       <c r="AB12" s="19"/>
-    </row>
-    <row r="13" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC12" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD12" s="19"/>
+      <c r="AE12" s="19"/>
+      <c r="AF12" s="19"/>
+    </row>
+    <row r="13" spans="2:32" ht="31.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="14" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C13" s="20">
         <v>180</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I13" s="17"/>
       <c r="J13" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="K13" s="17"/>
       <c r="L13" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="M13" s="17"/>
       <c r="N13" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="O13" s="17"/>
       <c r="P13" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="Q13" s="17"/>
       <c r="R13" s="18"/>
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
+      <c r="U13" s="18" t="s">
+        <v>114</v>
+      </c>
       <c r="V13" s="18"/>
       <c r="W13" s="18"/>
-      <c r="X13" s="19"/>
-      <c r="Y13" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z13" s="19"/>
-      <c r="AA13" s="19"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="18"/>
+      <c r="AA13" s="18"/>
       <c r="AB13" s="19"/>
-    </row>
-    <row r="14" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC13" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD13" s="19"/>
+      <c r="AE13" s="19"/>
+      <c r="AF13" s="19"/>
+    </row>
+    <row r="14" spans="2:32" ht="31.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="14" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C14" s="14">
         <v>45</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I14" s="17"/>
       <c r="J14" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
       <c r="M14" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="O14" s="17"/>
       <c r="P14" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="Q14" s="17"/>
       <c r="R14" s="18"/>
       <c r="S14" s="18"/>
       <c r="T14" s="18"/>
       <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
+      <c r="V14" s="18" t="s">
+        <v>114</v>
+      </c>
       <c r="W14" s="18"/>
-      <c r="X14" s="19"/>
-      <c r="Y14" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z14" s="19"/>
-      <c r="AA14" s="19"/>
+      <c r="X14" s="18"/>
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="18"/>
+      <c r="AA14" s="18"/>
       <c r="AB14" s="19"/>
-    </row>
-    <row r="15" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC14" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD14" s="19"/>
+      <c r="AE14" s="19"/>
+      <c r="AF14" s="19"/>
+    </row>
+    <row r="15" spans="2:32" ht="31.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="14" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C15" s="14">
         <v>93723</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J15" s="17"/>
       <c r="K15" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L15" s="17"/>
       <c r="M15" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="N15" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="O15" s="17"/>
       <c r="P15" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="Q15" s="17"/>
       <c r="R15" s="18"/>
@@ -3289,50 +3476,56 @@
       <c r="T15" s="18"/>
       <c r="U15" s="18"/>
       <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="19"/>
-      <c r="Y15" s="19"/>
-      <c r="Z15" s="19"/>
-      <c r="AA15" s="19"/>
-      <c r="AB15" s="19" t="s">
+      <c r="W15" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="18"/>
+      <c r="AA15" s="18"/>
+      <c r="AB15" s="19"/>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="19"/>
+      <c r="AE15" s="19"/>
+      <c r="AF15" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="14" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="14" t="s">
-        <v>125</v>
       </c>
       <c r="C16" s="14">
         <v>93680</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
       <c r="K16" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="M16" s="17"/>
       <c r="N16" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="O16" s="17"/>
       <c r="P16" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="Q16" s="17"/>
       <c r="R16" s="18"/>
@@ -3341,100 +3534,112 @@
       <c r="U16" s="18"/>
       <c r="V16" s="18"/>
       <c r="W16" s="18"/>
-      <c r="X16" s="19"/>
-      <c r="Y16" s="19"/>
-      <c r="Z16" s="19"/>
-      <c r="AA16" s="19" t="s">
-        <v>119</v>
-      </c>
+      <c r="X16" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y16" s="18"/>
+      <c r="Z16" s="18"/>
+      <c r="AA16" s="18"/>
       <c r="AB16" s="19"/>
-    </row>
-    <row r="17" spans="2:28" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC16" s="19"/>
+      <c r="AD16" s="19"/>
+      <c r="AE16" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF16" s="19"/>
+    </row>
+    <row r="17" spans="2:32" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="14" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C17" s="14">
         <v>-100</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
       <c r="I17" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J17" s="17"/>
       <c r="K17" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L17" s="17"/>
       <c r="M17" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="N17" s="17"/>
       <c r="O17" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="P17" s="17"/>
       <c r="Q17" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="R17" s="18"/>
+        <v>114</v>
+      </c>
+      <c r="R17" s="18" t="s">
+        <v>114</v>
+      </c>
       <c r="S17" s="18"/>
       <c r="T17" s="18"/>
       <c r="U17" s="18"/>
       <c r="V17" s="18"/>
       <c r="W17" s="18"/>
-      <c r="X17" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y17" s="19"/>
-      <c r="Z17" s="19"/>
-      <c r="AA17" s="19"/>
-      <c r="AB17" s="19"/>
-    </row>
-    <row r="18" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="X17" s="18"/>
+      <c r="Y17" s="18"/>
+      <c r="Z17" s="18"/>
+      <c r="AA17" s="18"/>
+      <c r="AB17" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC17" s="19"/>
+      <c r="AD17" s="19"/>
+      <c r="AE17" s="19"/>
+      <c r="AF17" s="19"/>
+    </row>
+    <row r="18" spans="2:32" ht="31.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="14" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C18" s="14">
         <v>86430</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J18" s="17"/>
       <c r="K18" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L18" s="17"/>
       <c r="M18" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="N18" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="O18" s="17"/>
       <c r="P18" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="Q18" s="17"/>
       <c r="R18" s="18"/>
@@ -3443,50 +3648,56 @@
       <c r="U18" s="18"/>
       <c r="V18" s="18"/>
       <c r="W18" s="18"/>
-      <c r="X18" s="19"/>
-      <c r="Y18" s="19"/>
-      <c r="Z18" s="19"/>
-      <c r="AA18" s="19"/>
-      <c r="AB18" s="19" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="2:28" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="X18" s="18"/>
+      <c r="Y18" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z18" s="18"/>
+      <c r="AA18" s="18"/>
+      <c r="AB18" s="19"/>
+      <c r="AC18" s="19"/>
+      <c r="AD18" s="19"/>
+      <c r="AE18" s="19"/>
+      <c r="AF18" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32" ht="31.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="14" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C19" s="14">
         <v>3660</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I19" s="17"/>
       <c r="J19" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="K19" s="17"/>
       <c r="L19" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="M19" s="17"/>
       <c r="N19" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="O19" s="17"/>
       <c r="P19" s="17"/>
       <c r="Q19" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="R19" s="18"/>
       <c r="S19" s="18"/>
@@ -3494,48 +3705,58 @@
       <c r="U19" s="18"/>
       <c r="V19" s="18"/>
       <c r="W19" s="18"/>
-      <c r="X19" s="19"/>
-      <c r="Y19" s="19"/>
-      <c r="Z19" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA19" s="19"/>
+      <c r="X19" s="18"/>
+      <c r="Y19" s="18"/>
+      <c r="Z19" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA19" s="18"/>
       <c r="AB19" s="19"/>
-    </row>
-    <row r="20" spans="2:28" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC19" s="19"/>
+      <c r="AD19" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE19" s="19"/>
+      <c r="AF19" s="19"/>
+    </row>
+    <row r="20" spans="2:32" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="X7:AB7"/>
-    <mergeCell ref="E6:AB6"/>
-    <mergeCell ref="AA8:AA9"/>
+  <mergeCells count="33">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:Q7"/>
+    <mergeCell ref="R7:AA7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="W8:W9"/>
+    <mergeCell ref="X8:X9"/>
+    <mergeCell ref="Y8:Y9"/>
+    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="AB7:AF7"/>
+    <mergeCell ref="E6:AF6"/>
+    <mergeCell ref="AE8:AE9"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="W8:W9"/>
+    <mergeCell ref="AA8:AA9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="Y8:Y9"/>
-    <mergeCell ref="Z8:Z9"/>
-    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="AC8:AC9"/>
+    <mergeCell ref="AD8:AD9"/>
+    <mergeCell ref="AF8:AF9"/>
     <mergeCell ref="V8:V9"/>
     <mergeCell ref="H8:I8"/>
-    <mergeCell ref="X8:X9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="U8:U9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:Q7"/>
-    <mergeCell ref="R7:W7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3570,63 +3791,63 @@
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="12"/>
-      <c r="D1" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="55"/>
+      <c r="D1" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="56"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="102" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="102"/>
-      <c r="K3" s="102"/>
-      <c r="L3" s="102"/>
+      <c r="B3" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="92" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="92" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="111" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="105" t="s">
+      <c r="D4" s="98" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="105" t="s">
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="106"/>
+      <c r="L4" s="88"/>
     </row>
     <row r="5" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B5" s="104"/>
-      <c r="C5" s="110"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="113" t="s">
+      <c r="B5" s="93"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114"/>
-      <c r="H5" s="114"/>
-      <c r="I5" s="114"/>
-      <c r="J5" s="115"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="102"/>
       <c r="K5" s="2" t="s">
         <v>4</v>
       </c>
@@ -3638,232 +3859,232 @@
       <c r="B6" s="23">
         <v>9</v>
       </c>
-      <c r="C6" s="107" t="s">
-        <v>36</v>
+      <c r="C6" s="94" t="s">
+        <v>34</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E6" s="121">
+        <v>125</v>
+      </c>
+      <c r="E6" s="108">
         <v>0</v>
       </c>
-      <c r="F6" s="122"/>
-      <c r="G6" s="122"/>
-      <c r="H6" s="122"/>
-      <c r="I6" s="122"/>
-      <c r="J6" s="123"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="110"/>
       <c r="K6" s="24" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="L6" s="23" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="23">
         <v>10</v>
       </c>
-      <c r="C7" s="107"/>
+      <c r="C7" s="94"/>
       <c r="D7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="105">
+        <v>40</v>
+      </c>
+      <c r="E7" s="86">
         <v>86400</v>
       </c>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="106"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="88"/>
       <c r="K7" s="23" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="23">
         <v>11</v>
       </c>
-      <c r="C8" s="107"/>
+      <c r="C8" s="94"/>
       <c r="D8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="105">
+        <v>41</v>
+      </c>
+      <c r="E8" s="86">
         <v>7200</v>
       </c>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="106"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="88"/>
       <c r="K8" s="23" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="23">
         <v>12</v>
       </c>
-      <c r="C9" s="107"/>
+      <c r="C9" s="94"/>
       <c r="D9" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E9" s="105">
+        <v>116</v>
+      </c>
+      <c r="E9" s="86">
         <v>180</v>
       </c>
-      <c r="F9" s="109"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="106"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="88"/>
       <c r="K9" s="23" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="L9" s="23" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="23">
         <v>13</v>
       </c>
-      <c r="C10" s="107"/>
+      <c r="C10" s="94"/>
       <c r="D10" s="52" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="105">
+        <v>117</v>
+      </c>
+      <c r="E10" s="86">
         <v>45</v>
       </c>
-      <c r="F10" s="109"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="109"/>
-      <c r="I10" s="109"/>
-      <c r="J10" s="106"/>
+      <c r="F10" s="87"/>
+      <c r="G10" s="87"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="88"/>
       <c r="K10" s="51" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="L10" s="51" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="23">
         <v>14</v>
       </c>
-      <c r="C11" s="107"/>
+      <c r="C11" s="94"/>
       <c r="D11" s="52" t="s">
-        <v>124</v>
-      </c>
-      <c r="E11" s="105">
+        <v>118</v>
+      </c>
+      <c r="E11" s="86">
         <v>93723</v>
       </c>
-      <c r="F11" s="109"/>
-      <c r="G11" s="109"/>
-      <c r="H11" s="109"/>
-      <c r="I11" s="109"/>
-      <c r="J11" s="106"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="88"/>
       <c r="K11" s="51" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="L11" s="51" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="23">
         <v>15</v>
       </c>
-      <c r="C12" s="107"/>
+      <c r="C12" s="94"/>
       <c r="D12" s="52" t="s">
-        <v>138</v>
-      </c>
-      <c r="E12" s="105">
+        <v>130</v>
+      </c>
+      <c r="E12" s="86">
         <v>86430</v>
       </c>
-      <c r="F12" s="109"/>
-      <c r="G12" s="109"/>
-      <c r="H12" s="109"/>
-      <c r="I12" s="109"/>
-      <c r="J12" s="106"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="88"/>
       <c r="K12" s="51" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="L12" s="51" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="23">
         <v>16</v>
       </c>
-      <c r="C13" s="107"/>
+      <c r="C13" s="94"/>
       <c r="D13" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" s="86">
+        <v>3660</v>
+      </c>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="L13" s="51" t="s">
         <v>139</v>
-      </c>
-      <c r="E13" s="105">
-        <v>3660</v>
-      </c>
-      <c r="F13" s="109"/>
-      <c r="G13" s="109"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="106"/>
-      <c r="K13" s="51" t="s">
-        <v>132</v>
-      </c>
-      <c r="L13" s="51" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="23">
         <v>17</v>
       </c>
-      <c r="C14" s="107"/>
+      <c r="C14" s="94"/>
       <c r="D14" s="52" t="s">
-        <v>125</v>
-      </c>
-      <c r="E14" s="105">
+        <v>119</v>
+      </c>
+      <c r="E14" s="86">
         <v>93680</v>
       </c>
-      <c r="F14" s="109"/>
-      <c r="G14" s="109"/>
-      <c r="H14" s="109"/>
-      <c r="I14" s="109"/>
-      <c r="J14" s="106"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="87"/>
+      <c r="I14" s="87"/>
+      <c r="J14" s="88"/>
       <c r="K14" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="L14" s="51" t="s">
         <v>136</v>
-      </c>
-      <c r="L14" s="51" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B15" s="23">
         <v>18</v>
       </c>
-      <c r="C15" s="108"/>
+      <c r="C15" s="95"/>
       <c r="D15" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E15" s="105">
+        <v>129</v>
+      </c>
+      <c r="E15" s="86">
         <v>-100</v>
       </c>
-      <c r="F15" s="109"/>
-      <c r="G15" s="109"/>
-      <c r="H15" s="109"/>
-      <c r="I15" s="109"/>
-      <c r="J15" s="106"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="88"/>
       <c r="K15" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
@@ -3881,88 +4102,88 @@
     </row>
     <row r="17" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B17" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K17" s="25"/>
     </row>
     <row r="18" spans="2:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B18" s="116" t="s">
+      <c r="B18" s="103" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="104"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="105" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="106"/>
+      <c r="H18" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="118" t="s">
+      <c r="I18" s="104"/>
+      <c r="J18" s="104"/>
+      <c r="K18" s="104"/>
+      <c r="L18" s="107"/>
+      <c r="M18" s="89" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="119"/>
-      <c r="H18" s="116" t="s">
+      <c r="N18" s="90"/>
+    </row>
+    <row r="19" spans="2:14" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="122" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="115" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="115" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="124" t="s">
         <v>59</v>
       </c>
-      <c r="I18" s="117"/>
-      <c r="J18" s="117"/>
-      <c r="K18" s="117"/>
-      <c r="L18" s="120"/>
-      <c r="M18" s="100" t="s">
+      <c r="F19" s="112" t="s">
         <v>60</v>
       </c>
-      <c r="N18" s="101"/>
-    </row>
-    <row r="19" spans="2:14" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="83" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="85" t="s">
+      <c r="G19" s="111" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="113" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="115" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="85" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="87" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="91" t="s">
+      <c r="L19" s="119" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="93" t="s">
+      <c r="M19" s="121" t="s">
         <v>64</v>
       </c>
-      <c r="I19" s="85" t="s">
-        <v>32</v>
-      </c>
-      <c r="J19" s="85" t="s">
-        <v>33</v>
-      </c>
-      <c r="K19" s="95" t="s">
-        <v>35</v>
-      </c>
-      <c r="L19" s="97" t="s">
+      <c r="N19" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="M19" s="99" t="s">
-        <v>66</v>
-      </c>
-      <c r="N19" s="92" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="20" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="84"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="90"/>
-      <c r="G20" s="91"/>
-      <c r="H20" s="94"/>
-      <c r="I20" s="86"/>
-      <c r="J20" s="86"/>
-      <c r="K20" s="96"/>
-      <c r="L20" s="98"/>
-      <c r="M20" s="83"/>
-      <c r="N20" s="89"/>
+      <c r="B20" s="123"/>
+      <c r="C20" s="116"/>
+      <c r="D20" s="116"/>
+      <c r="E20" s="125"/>
+      <c r="F20" s="126"/>
+      <c r="G20" s="111"/>
+      <c r="H20" s="114"/>
+      <c r="I20" s="116"/>
+      <c r="J20" s="116"/>
+      <c r="K20" s="118"/>
+      <c r="L20" s="120"/>
+      <c r="M20" s="122"/>
+      <c r="N20" s="112"/>
     </row>
     <row r="21" spans="2:14" ht="41.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="29">
@@ -3976,7 +4197,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="F21" s="28">
         <v>2</v>
@@ -3985,7 +4206,7 @@
         <v>2</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="I21" s="29">
         <v>9</v>
@@ -3997,10 +4218,10 @@
         <v>2</v>
       </c>
       <c r="L21" s="31" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="N21" s="32">
         <f>C21</f>
@@ -4009,13 +4230,19 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:L3"/>
@@ -4032,19 +4259,13 @@
     <mergeCell ref="E6:J6"/>
     <mergeCell ref="E7:J7"/>
     <mergeCell ref="E8:J8"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="E13:J13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4052,15 +4273,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5F472198D7887469049920058585067" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e76e8f6ca957e849a493f1baa4f4bb7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c46c0853-0d59-45c6-b517-3e25eac8cdf1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ddeb00cc2097713d6f56fe4f26be38f" ns2:_="">
     <xsd:import namespace="c46c0853-0d59-45c6-b517-3e25eac8cdf1"/>
@@ -4204,6 +4416,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -4211,14 +4432,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E53DB3A-2750-466D-B803-7A1FAB16D24B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4236,6 +4449,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC4FB184-C14D-4C2C-BD91-7F8240B2478B}">
   <ds:schemaRefs>

</xml_diff>